<commit_message>
added a preceding bidirectional layer
</commit_message>
<xml_diff>
--- a/hw2sent/dictionary_size.xlsx
+++ b/hw2sent/dictionary_size.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dawesl\Documents\Computing\comp9444\hw2\hw2sent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldawe\Documents\computing\comp9444\hw2\hw2sent\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>best accuracy</t>
   </si>
@@ -40,15 +40,59 @@
   <si>
     <t>but solid</t>
   </si>
+  <si>
+    <t>stopword size</t>
+  </si>
+  <si>
+    <t>original stoplist</t>
+  </si>
+  <si>
+    <t>several unchanged runs</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>95% ci</t>
+  </si>
+  <si>
+    <t>ci</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,14 +118,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -98,7 +148,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -145,7 +195,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -286,6 +335,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7CB2-44EC-B29F-5A503F5EF80E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -470,7 +524,390 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>stopwords vs accuracy</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$18:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.72412434683500004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.74241172013599999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74545020247399996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.74803724755199996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.74603461523500003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74518293676699998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C561-46EF-A2D0-7B7CA8AD6BC2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="583500728"/>
+        <c:axId val="583501712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="583500728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="583501712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="583501712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="583500728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1026,24 +1463,546 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>430530</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>125730</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1053,6 +2012,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>423862</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{178C403C-53DD-417B-8D35-FB26288A87BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1323,127 +2318,326 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="12.28515625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>0.54400000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>100</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>0.60840000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>1000</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>0.69289999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>10000</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>0.74070000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>30000</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>0.7641</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>50000</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>0.76370000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>100000</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>0.76280000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>400000</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>0.7591</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>0.79200000000000004</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>100</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>0.75880000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>1000</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>0.74429999999999996</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.72412434683500004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.74241172013599999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.74545020247399996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.74803724755199996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>50</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.74603461523500003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>105</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.74518293676699998</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>0.74707406239724605</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>0.75309893739478495</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>0.73840862174273303</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>0.74183443189799703</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>0.74514268302520204</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>0.74987574438206495</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <v>0.73907966071962905</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <v>0.74678226691153105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>0.75759231994884202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <v>0.73683805858734897</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
+        <v>0.75029005888959799</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>0.75567646759437601</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="2">
+        <v>0.75103040599762005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="2">
+        <v>0.74484140511220198</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="2">
+        <v>0.74877856230955897</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="2">
+        <v>0.73608020972899302</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="2">
+        <v>0.75076528391647301</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="2">
+        <v>0.74856817186343305</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
+        <v>0.74820805904021603</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="5">
+        <f>AVERAGE(B26:B44)</f>
+        <v>0.74684028481367637</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="5">
+        <f>_xlfn.STDEV.S(B26:B44)</f>
+        <v>6.1222910292293535E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="2">
+        <f>B45-_xlfn.CONFIDENCE.T(0.05,B46,COUNT(B26:B44))</f>
+        <v>0.74388943499433413</v>
+      </c>
+      <c r="C47" s="2">
+        <f>B45 + _xlfn.CONFIDENCE.T(0.05,B46,COUNT(B26:B44))</f>
+        <v>0.74979113463301861</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="3">
+        <f>_xlfn.CONFIDENCE.T(0.05,B46,COUNT(B26:B44))</f>
+        <v>2.9508498193422071E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>